<commit_message>
Added source code for dvwa, and the llmfileprocessor class
</commit_message>
<xml_diff>
--- a/vulnerable_applications/ApplicationTracker.xlsx
+++ b/vulnerable_applications/ApplicationTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\myagents\vulnerable_applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED1D00D-B7AF-4F5B-B763-2D3CCC5ABC06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD7C016-51E3-4B9E-87C4-FE0A5BA2E830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{5948C3E8-F7AB-40EB-BB76-DA3AF29A7BC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="44">
   <si>
     <t>Application</t>
   </si>
@@ -150,6 +150,24 @@
   </si>
   <si>
     <t>Mermaid</t>
+  </si>
+  <si>
+    <t>Known Vulnerabilities</t>
+  </si>
+  <si>
+    <t>Found by Agent</t>
+  </si>
+  <si>
+    <t>OWASPVulnerable_app</t>
+  </si>
+  <si>
+    <t>Known Vulns</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -219,11 +237,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -560,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A0B659-7FDF-4553-AEEC-A88C41F596EC}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -572,9 +599,10 @@
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="13.19921875" customWidth="1"/>
     <col min="4" max="5" width="13.06640625" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,8 +621,17 @@
       <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -610,11 +647,17 @@
       <c r="E2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -633,8 +676,14 @@
       <c r="F3" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -653,8 +702,14 @@
       <c r="F4" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -673,8 +728,14 @@
       <c r="F5" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -693,8 +754,11 @@
       <c r="F6" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -713,8 +777,11 @@
       <c r="F7" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -733,8 +800,14 @@
       <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -753,8 +826,11 @@
       <c r="F9" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -773,8 +849,11 @@
       <c r="F10" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -793,8 +872,11 @@
       <c r="F11" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G11" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -813,8 +895,11 @@
       <c r="F12" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -833,8 +918,14 @@
       <c r="F13" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -853,8 +944,11 @@
       <c r="F14" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G14" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -873,8 +967,11 @@
       <c r="F15" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G15" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -893,8 +990,11 @@
       <c r="F16" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -913,8 +1013,11 @@
       <c r="F17" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -933,8 +1036,11 @@
       <c r="F18" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G18" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -953,8 +1059,11 @@
       <c r="F19" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G19" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -973,8 +1082,11 @@
       <c r="F20" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G20" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -993,8 +1105,14 @@
       <c r="F21" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1013,8 +1131,14 @@
       <c r="F22" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1033,8 +1157,14 @@
       <c r="F23" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1053,8 +1183,11 @@
       <c r="F24" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G24" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1073,8 +1206,14 @@
       <c r="F25" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1093,8 +1232,11 @@
       <c r="F26" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G26" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1113,8 +1255,11 @@
       <c r="F27" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G27" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1133,8 +1278,11 @@
       <c r="F28" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G28" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1153,8 +1301,14 @@
       <c r="F29" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1173,8 +1327,11 @@
       <c r="F30" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G30" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1193,6 +1350,126 @@
       <c r="F31" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="G31" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="5">
+        <v>13</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="5">
+        <v>10</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="5">
+        <v>14</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="5">
+        <v>14</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="5">
+        <v>65</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="5">
+        <v>25</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="5">
+        <v>65</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="5">
+        <v>45</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="5">
+        <v>50</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="5">
+        <v>50</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="5">
+        <v>25</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>